<commit_message>
i360--upload and corescript update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/analysis_00_ta_engine.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/analysis_00_ta_engine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\TMP_EIT_suites\radiant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
@@ -27,10 +27,10 @@
   </definedNames>
   <calcPr calcId="122211" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
+    <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1557,10 +1557,10 @@
     <t>flow</t>
   </si>
   <si>
-    <t>cmd = python DEV/bin/run_radiant.py --synthesis=lse --run-par-trce --run-par-iota</t>
-  </si>
-  <si>
-    <t>analysis_00_ta_engine_v2.00</t>
+    <t>cmd = python DEV/bin/run_radiant.py --synthesis=lse  --run-synthesis-trce --run-map-trce --run-par-trce --run-par-iota</t>
+  </si>
+  <si>
+    <t>analysis_00_ta_engine_v2.01</t>
   </si>
 </sst>
 </file>
@@ -2863,31 +2863,64 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2899,13 +2932,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2925,44 +2952,17 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -5465,7 +5465,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4A90B330-1C2F-4F83-8484-9D7B950E9A8A}" diskRevisions="1" revisionId="545" version="5">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{ED524B24-CBD6-4052-80C8-598B3FD1E581}" diskRevisions="1" revisionId="547" version="7">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5506,6 +5506,22 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{03E03F4C-C462-4948-BFE1-85F5FA05FB70}" dateTime="2021-07-28T15:41:27" maxSheetId="5" userName="Jason Wang" r:id="rId6" minRId="546">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{ED524B24-CBD6-4052-80C8-598B3FD1E581}" dateTime="2021-07-28T15:41:49" maxSheetId="5" userName="Jason Wang" r:id="rId7" minRId="547">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -9502,7 +9518,41 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="546" sId="1">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>cmd = python DEV/bin/run_radiant.py --synthesis=lse --run-par-trce --run-par-iota</t>
+      </is>
+    </oc>
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>cmd = python DEV/bin/run_radiant.py --synthesis=lse  --run-synthesis-trce --run-map-trce --run-par-trce --run-par-iota</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="547" sId="1">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>analysis_00_ta_engine_v2.00</t>
+      </is>
+    </oc>
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>analysis_00_ta_engine_v2.01</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" name="Cherry (Ying) Xu" id="-707422276" dateTime="2020-11-23T15:52:35"/>
 </users>
@@ -9798,7 +9848,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -9884,23 +9934,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B23" sqref="B23"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
       <selection activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B23" sqref="B23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -11831,33 +11881,33 @@
   <sheetProtection algorithmName="SHA-512" hashValue="y+CBG6/YKaQ6HsaQYTqaGGAc9K7SdI4KYNN5n42I5k04yiTX0Fn8xQwrYnwNAtl9mwRmr3UcHPCrpySoPgBJNA==" saltValue="2QS/OSgjoJCpqDc5Ec8Idw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AD2"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="70" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AF11" sqref="AF11"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:AD2"/>
+      <autoFilter ref="A2:Y2"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A2:Y2"/>
     </customSheetView>
     <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="70" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="A109" sqref="A109:XFD109"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A2:AD2"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:Y2"/>
-    </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="70" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AF11" sqref="AF11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AD2"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -11998,17 +12048,17 @@
       <c r="E111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F111" s="73" t="s">
+      <c r="F111" s="104" t="s">
         <v>87</v>
       </c>
-      <c r="G111" s="74"/>
-      <c r="H111" s="74"/>
-      <c r="I111" s="74"/>
-      <c r="J111" s="74"/>
-      <c r="K111" s="74"/>
-      <c r="L111" s="74"/>
-      <c r="M111" s="74"/>
-      <c r="N111" s="75"/>
+      <c r="G111" s="105"/>
+      <c r="H111" s="105"/>
+      <c r="I111" s="105"/>
+      <c r="J111" s="105"/>
+      <c r="K111" s="105"/>
+      <c r="L111" s="105"/>
+      <c r="M111" s="105"/>
+      <c r="N111" s="106"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -12872,7 +12922,7 @@
       <c r="A147" s="26">
         <v>1</v>
       </c>
-      <c r="B147" s="76" t="s">
+      <c r="B147" s="89" t="s">
         <v>3</v>
       </c>
       <c r="C147" s="27" t="s">
@@ -12898,7 +12948,7 @@
       <c r="A148" s="26">
         <v>2</v>
       </c>
-      <c r="B148" s="77"/>
+      <c r="B148" s="90"/>
       <c r="C148" s="28" t="s">
         <v>136</v>
       </c>
@@ -12920,7 +12970,7 @@
       <c r="A149" s="26">
         <v>3</v>
       </c>
-      <c r="B149" s="77"/>
+      <c r="B149" s="90"/>
       <c r="C149" s="28" t="s">
         <v>9</v>
       </c>
@@ -12940,7 +12990,7 @@
       <c r="A150" s="26">
         <v>4</v>
       </c>
-      <c r="B150" s="77"/>
+      <c r="B150" s="90"/>
       <c r="C150" s="28" t="s">
         <v>138</v>
       </c>
@@ -12964,7 +13014,7 @@
       <c r="A151" s="26">
         <v>5</v>
       </c>
-      <c r="B151" s="77"/>
+      <c r="B151" s="90"/>
       <c r="C151" s="27" t="s">
         <v>140</v>
       </c>
@@ -12988,7 +13038,7 @@
       <c r="A152" s="26">
         <v>6</v>
       </c>
-      <c r="B152" s="77"/>
+      <c r="B152" s="90"/>
       <c r="C152" s="27" t="s">
         <v>144</v>
       </c>
@@ -13012,7 +13062,7 @@
       <c r="A153" s="26">
         <v>7</v>
       </c>
-      <c r="B153" s="77"/>
+      <c r="B153" s="90"/>
       <c r="C153" s="28" t="s">
         <v>147</v>
       </c>
@@ -13034,7 +13084,7 @@
       <c r="A154" s="26">
         <v>8</v>
       </c>
-      <c r="B154" s="77"/>
+      <c r="B154" s="90"/>
       <c r="C154" s="27" t="s">
         <v>148</v>
       </c>
@@ -13058,7 +13108,7 @@
       <c r="A155" s="26">
         <v>9</v>
       </c>
-      <c r="B155" s="77"/>
+      <c r="B155" s="90"/>
       <c r="C155" s="27" t="s">
         <v>149</v>
       </c>
@@ -13082,7 +13132,7 @@
       <c r="A156" s="26">
         <v>10</v>
       </c>
-      <c r="B156" s="77"/>
+      <c r="B156" s="90"/>
       <c r="C156" s="28" t="s">
         <v>150</v>
       </c>
@@ -13106,7 +13156,7 @@
       <c r="A157" s="26">
         <v>11</v>
       </c>
-      <c r="B157" s="77"/>
+      <c r="B157" s="90"/>
       <c r="C157" s="28" t="s">
         <v>151</v>
       </c>
@@ -13130,7 +13180,7 @@
       <c r="A158" s="26">
         <v>12</v>
       </c>
-      <c r="B158" s="77"/>
+      <c r="B158" s="90"/>
       <c r="C158" s="28" t="s">
         <v>153</v>
       </c>
@@ -13152,7 +13202,7 @@
       <c r="A159" s="26">
         <v>13</v>
       </c>
-      <c r="B159" s="78"/>
+      <c r="B159" s="84"/>
       <c r="C159" s="28" t="s">
         <v>56</v>
       </c>
@@ -13176,7 +13226,7 @@
       <c r="A160" s="26">
         <v>14</v>
       </c>
-      <c r="B160" s="71" t="s">
+      <c r="B160" s="80" t="s">
         <v>4</v>
       </c>
       <c r="C160" s="28" t="s">
@@ -13202,7 +13252,7 @@
       <c r="A161" s="26">
         <v>15</v>
       </c>
-      <c r="B161" s="72"/>
+      <c r="B161" s="79"/>
       <c r="C161" s="28" t="s">
         <v>161</v>
       </c>
@@ -13226,7 +13276,7 @@
       <c r="A162" s="26">
         <v>16</v>
       </c>
-      <c r="B162" s="76" t="s">
+      <c r="B162" s="89" t="s">
         <v>5</v>
       </c>
       <c r="C162" s="28" t="s">
@@ -13250,7 +13300,7 @@
       <c r="A163" s="26">
         <v>17</v>
       </c>
-      <c r="B163" s="79"/>
+      <c r="B163" s="107"/>
       <c r="C163" s="27" t="s">
         <v>165</v>
       </c>
@@ -13272,7 +13322,7 @@
       <c r="A164" s="26">
         <v>18</v>
       </c>
-      <c r="B164" s="78"/>
+      <c r="B164" s="84"/>
       <c r="C164" s="27" t="s">
         <v>167</v>
       </c>
@@ -13292,7 +13342,7 @@
       <c r="A165" s="26">
         <v>19</v>
       </c>
-      <c r="B165" s="71" t="s">
+      <c r="B165" s="80" t="s">
         <v>6</v>
       </c>
       <c r="C165" s="28" t="s">
@@ -13316,7 +13366,7 @@
       <c r="A166" s="26">
         <v>20</v>
       </c>
-      <c r="B166" s="72"/>
+      <c r="B166" s="79"/>
       <c r="C166" s="28" t="s">
         <v>172</v>
       </c>
@@ -13336,7 +13386,7 @@
       <c r="A167" s="26">
         <v>21</v>
       </c>
-      <c r="B167" s="72"/>
+      <c r="B167" s="79"/>
       <c r="C167" s="28" t="s">
         <v>173</v>
       </c>
@@ -13356,7 +13406,7 @@
       <c r="A168" s="26">
         <v>22</v>
       </c>
-      <c r="B168" s="72"/>
+      <c r="B168" s="79"/>
       <c r="C168" s="28" t="s">
         <v>174</v>
       </c>
@@ -13376,7 +13426,7 @@
       <c r="A169" s="26">
         <v>23</v>
       </c>
-      <c r="B169" s="72"/>
+      <c r="B169" s="79"/>
       <c r="C169" s="28" t="s">
         <v>175</v>
       </c>
@@ -13396,7 +13446,7 @@
       <c r="A170" s="26">
         <v>24</v>
       </c>
-      <c r="B170" s="72"/>
+      <c r="B170" s="79"/>
       <c r="C170" s="28" t="s">
         <v>176</v>
       </c>
@@ -13416,7 +13466,7 @@
       <c r="A171" s="26">
         <v>25</v>
       </c>
-      <c r="B171" s="72"/>
+      <c r="B171" s="79"/>
       <c r="C171" s="28" t="s">
         <v>177</v>
       </c>
@@ -13436,7 +13486,7 @@
       <c r="A172" s="26">
         <v>26</v>
       </c>
-      <c r="B172" s="72"/>
+      <c r="B172" s="79"/>
       <c r="C172" s="28" t="s">
         <v>41</v>
       </c>
@@ -13456,7 +13506,7 @@
       <c r="A173" s="26">
         <v>27</v>
       </c>
-      <c r="B173" s="71" t="s">
+      <c r="B173" s="80" t="s">
         <v>7</v>
       </c>
       <c r="C173" s="28" t="s">
@@ -13480,7 +13530,7 @@
       <c r="A174" s="26">
         <v>28</v>
       </c>
-      <c r="B174" s="72"/>
+      <c r="B174" s="79"/>
       <c r="C174" s="27" t="s">
         <v>181</v>
       </c>
@@ -13502,7 +13552,7 @@
       <c r="A175" s="26">
         <v>29</v>
       </c>
-      <c r="B175" s="72"/>
+      <c r="B175" s="79"/>
       <c r="C175" s="28" t="s">
         <v>184</v>
       </c>
@@ -13524,7 +13574,7 @@
       <c r="A176" s="26">
         <v>30</v>
       </c>
-      <c r="B176" s="76" t="s">
+      <c r="B176" s="89" t="s">
         <v>8</v>
       </c>
       <c r="C176" s="28" t="s">
@@ -13550,7 +13600,7 @@
       <c r="A177" s="31">
         <v>31</v>
       </c>
-      <c r="B177" s="77"/>
+      <c r="B177" s="90"/>
       <c r="C177" s="32" t="s">
         <v>189</v>
       </c>
@@ -13574,7 +13624,7 @@
       <c r="A178" s="23">
         <v>32</v>
       </c>
-      <c r="B178" s="80" t="s">
+      <c r="B178" s="91" t="s">
         <v>191</v>
       </c>
       <c r="C178" s="33" t="s">
@@ -13598,7 +13648,7 @@
       <c r="A179" s="26">
         <v>33</v>
       </c>
-      <c r="B179" s="81"/>
+      <c r="B179" s="92"/>
       <c r="C179" s="27" t="s">
         <v>195</v>
       </c>
@@ -13620,7 +13670,7 @@
       <c r="A180" s="26">
         <v>34</v>
       </c>
-      <c r="B180" s="82"/>
+      <c r="B180" s="93"/>
       <c r="C180" s="34" t="s">
         <v>198</v>
       </c>
@@ -13642,7 +13692,7 @@
       <c r="A181" s="31">
         <v>35</v>
       </c>
-      <c r="B181" s="82"/>
+      <c r="B181" s="93"/>
       <c r="C181" s="34" t="s">
         <v>199</v>
       </c>
@@ -13664,7 +13714,7 @@
       <c r="A182" s="31">
         <v>36</v>
       </c>
-      <c r="B182" s="82"/>
+      <c r="B182" s="93"/>
       <c r="C182" s="34" t="s">
         <v>202</v>
       </c>
@@ -13684,7 +13734,7 @@
       <c r="A183" s="31">
         <v>37</v>
       </c>
-      <c r="B183" s="82"/>
+      <c r="B183" s="93"/>
       <c r="C183" s="34" t="s">
         <v>254</v>
       </c>
@@ -13706,7 +13756,7 @@
       <c r="A184" s="35">
         <v>38</v>
       </c>
-      <c r="B184" s="83"/>
+      <c r="B184" s="88"/>
       <c r="C184" s="36" t="s">
         <v>258</v>
       </c>
@@ -13757,11 +13807,11 @@
       <c r="B198" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C198" s="84" t="s">
+      <c r="C198" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="D198" s="84"/>
-      <c r="E198" s="84"/>
+      <c r="D198" s="94"/>
+      <c r="E198" s="94"/>
       <c r="F198" s="39" t="s">
         <v>43</v>
       </c>
@@ -13770,17 +13820,17 @@
       </c>
     </row>
     <row r="199" spans="1:7">
-      <c r="A199" s="85" t="s">
+      <c r="A199" s="77" t="s">
         <v>212</v>
       </c>
-      <c r="B199" s="72" t="s">
+      <c r="B199" s="79" t="s">
         <v>213</v>
       </c>
-      <c r="C199" s="87" t="s">
+      <c r="C199" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="D199" s="88"/>
-      <c r="E199" s="88"/>
+      <c r="D199" s="97"/>
+      <c r="E199" s="97"/>
       <c r="F199" s="28" t="s">
         <v>214</v>
       </c>
@@ -13789,13 +13839,13 @@
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="85"/>
-      <c r="B200" s="86"/>
-      <c r="C200" s="89" t="s">
+      <c r="A200" s="77"/>
+      <c r="B200" s="95"/>
+      <c r="C200" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="D200" s="90"/>
-      <c r="E200" s="90"/>
+      <c r="D200" s="99"/>
+      <c r="E200" s="99"/>
       <c r="F200" s="32" t="s">
         <v>215</v>
       </c>
@@ -13804,15 +13854,15 @@
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="85"/>
-      <c r="B201" s="72" t="s">
+      <c r="A201" s="77"/>
+      <c r="B201" s="79" t="s">
         <v>216</v>
       </c>
-      <c r="C201" s="91" t="s">
+      <c r="C201" s="100" t="s">
         <v>217</v>
       </c>
-      <c r="D201" s="91"/>
-      <c r="E201" s="91"/>
+      <c r="D201" s="100"/>
+      <c r="E201" s="100"/>
       <c r="F201" s="28" t="s">
         <v>214</v>
       </c>
@@ -13821,13 +13871,13 @@
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="85"/>
-      <c r="B202" s="72"/>
-      <c r="C202" s="89" t="s">
+      <c r="A202" s="77"/>
+      <c r="B202" s="79"/>
+      <c r="C202" s="98" t="s">
         <v>217</v>
       </c>
-      <c r="D202" s="89"/>
-      <c r="E202" s="89"/>
+      <c r="D202" s="98"/>
+      <c r="E202" s="98"/>
       <c r="F202" s="28" t="s">
         <v>215</v>
       </c>
@@ -13836,15 +13886,15 @@
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="85"/>
-      <c r="B203" s="86" t="s">
+      <c r="A203" s="77"/>
+      <c r="B203" s="95" t="s">
         <v>218</v>
       </c>
-      <c r="C203" s="92" t="s">
+      <c r="C203" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="D203" s="93"/>
-      <c r="E203" s="94"/>
+      <c r="D203" s="102"/>
+      <c r="E203" s="103"/>
       <c r="F203" s="28" t="s">
         <v>214</v>
       </c>
@@ -13853,13 +13903,13 @@
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="85"/>
-      <c r="B204" s="78"/>
-      <c r="C204" s="92" t="s">
+      <c r="A204" s="77"/>
+      <c r="B204" s="84"/>
+      <c r="C204" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="93"/>
-      <c r="E204" s="94"/>
+      <c r="D204" s="102"/>
+      <c r="E204" s="103"/>
       <c r="F204" s="28" t="s">
         <v>215</v>
       </c>
@@ -13868,15 +13918,15 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="85"/>
-      <c r="B205" s="72" t="s">
+      <c r="A205" s="77"/>
+      <c r="B205" s="79" t="s">
         <v>219</v>
       </c>
-      <c r="C205" s="91" t="s">
+      <c r="C205" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="D205" s="91"/>
-      <c r="E205" s="91"/>
+      <c r="D205" s="100"/>
+      <c r="E205" s="100"/>
       <c r="F205" s="28" t="s">
         <v>214</v>
       </c>
@@ -13885,13 +13935,13 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="85"/>
-      <c r="B206" s="72"/>
-      <c r="C206" s="91" t="s">
+      <c r="A206" s="77"/>
+      <c r="B206" s="79"/>
+      <c r="C206" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="D206" s="91"/>
-      <c r="E206" s="91"/>
+      <c r="D206" s="100"/>
+      <c r="E206" s="100"/>
       <c r="F206" s="28" t="s">
         <v>215</v>
       </c>
@@ -13900,17 +13950,17 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="85" t="s">
+      <c r="A207" s="77" t="s">
         <v>221</v>
       </c>
-      <c r="B207" s="72" t="s">
+      <c r="B207" s="79" t="s">
         <v>222</v>
       </c>
-      <c r="C207" s="71" t="s">
+      <c r="C207" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="D207" s="72"/>
-      <c r="E207" s="72"/>
+      <c r="D207" s="79"/>
+      <c r="E207" s="79"/>
       <c r="F207" s="28" t="s">
         <v>214</v>
       </c>
@@ -13919,13 +13969,13 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="85"/>
-      <c r="B208" s="72"/>
-      <c r="C208" s="72" t="s">
+      <c r="A208" s="77"/>
+      <c r="B208" s="79"/>
+      <c r="C208" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="D208" s="72"/>
-      <c r="E208" s="72"/>
+      <c r="D208" s="79"/>
+      <c r="E208" s="79"/>
       <c r="F208" s="28" t="s">
         <v>215</v>
       </c>
@@ -13934,15 +13984,15 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="85"/>
-      <c r="B209" s="72" t="s">
+      <c r="A209" s="77"/>
+      <c r="B209" s="79" t="s">
         <v>224</v>
       </c>
-      <c r="C209" s="72" t="s">
+      <c r="C209" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="D209" s="72"/>
-      <c r="E209" s="72"/>
+      <c r="D209" s="79"/>
+      <c r="E209" s="79"/>
       <c r="F209" s="28" t="s">
         <v>214</v>
       </c>
@@ -13951,13 +14001,13 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="85"/>
-      <c r="B210" s="72"/>
-      <c r="C210" s="72" t="s">
+      <c r="A210" s="77"/>
+      <c r="B210" s="79"/>
+      <c r="C210" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="D210" s="72"/>
-      <c r="E210" s="72"/>
+      <c r="D210" s="79"/>
+      <c r="E210" s="79"/>
       <c r="F210" s="28" t="s">
         <v>215</v>
       </c>
@@ -13966,17 +14016,17 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="85" t="s">
+      <c r="A211" s="77" t="s">
         <v>225</v>
       </c>
-      <c r="B211" s="72" t="s">
+      <c r="B211" s="79" t="s">
         <v>226</v>
       </c>
-      <c r="C211" s="71" t="s">
+      <c r="C211" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="D211" s="72"/>
-      <c r="E211" s="72"/>
+      <c r="D211" s="79"/>
+      <c r="E211" s="79"/>
       <c r="F211" s="28" t="s">
         <v>214</v>
       </c>
@@ -13985,13 +14035,13 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="85"/>
-      <c r="B212" s="72"/>
-      <c r="C212" s="72" t="s">
+      <c r="A212" s="77"/>
+      <c r="B212" s="79"/>
+      <c r="C212" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="D212" s="72"/>
-      <c r="E212" s="72"/>
+      <c r="D212" s="79"/>
+      <c r="E212" s="79"/>
       <c r="F212" s="28" t="s">
         <v>215</v>
       </c>
@@ -14000,15 +14050,15 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="85"/>
-      <c r="B213" s="72" t="s">
+      <c r="A213" s="77"/>
+      <c r="B213" s="79" t="s">
         <v>227</v>
       </c>
-      <c r="C213" s="71" t="s">
+      <c r="C213" s="80" t="s">
         <v>228</v>
       </c>
-      <c r="D213" s="72"/>
-      <c r="E213" s="72"/>
+      <c r="D213" s="79"/>
+      <c r="E213" s="79"/>
       <c r="F213" s="28" t="s">
         <v>214</v>
       </c>
@@ -14017,13 +14067,13 @@
       </c>
     </row>
     <row r="214" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A214" s="96"/>
-      <c r="B214" s="97"/>
-      <c r="C214" s="97" t="s">
+      <c r="A214" s="78"/>
+      <c r="B214" s="81"/>
+      <c r="C214" s="81" t="s">
         <v>229</v>
       </c>
-      <c r="D214" s="97"/>
-      <c r="E214" s="97"/>
+      <c r="D214" s="81"/>
+      <c r="E214" s="81"/>
       <c r="F214" s="36" t="s">
         <v>215</v>
       </c>
@@ -14062,12 +14112,12 @@
       <c r="A219" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="B219" s="98" t="s">
+      <c r="B219" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="C219" s="98"/>
-      <c r="D219" s="98"/>
-      <c r="E219" s="98"/>
+      <c r="C219" s="82"/>
+      <c r="D219" s="82"/>
+      <c r="E219" s="82"/>
       <c r="F219" s="46" t="s">
         <v>233</v>
       </c>
@@ -14079,12 +14129,12 @@
       <c r="A220" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="B220" s="99" t="s">
+      <c r="B220" s="83" t="s">
         <v>236</v>
       </c>
-      <c r="C220" s="78"/>
-      <c r="D220" s="78"/>
-      <c r="E220" s="78"/>
+      <c r="C220" s="84"/>
+      <c r="D220" s="84"/>
+      <c r="E220" s="84"/>
       <c r="F220" s="49" t="s">
         <v>111</v>
       </c>
@@ -14096,12 +14146,12 @@
       <c r="A221" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B221" s="100" t="s">
+      <c r="B221" s="85" t="s">
         <v>238</v>
       </c>
-      <c r="C221" s="101"/>
-      <c r="D221" s="101"/>
-      <c r="E221" s="102"/>
+      <c r="C221" s="86"/>
+      <c r="D221" s="86"/>
+      <c r="E221" s="87"/>
       <c r="F221" s="15" t="s">
         <v>63</v>
       </c>
@@ -14113,12 +14163,12 @@
       <c r="A222" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B222" s="100" t="s">
+      <c r="B222" s="85" t="s">
         <v>239</v>
       </c>
-      <c r="C222" s="101"/>
-      <c r="D222" s="101"/>
-      <c r="E222" s="102"/>
+      <c r="C222" s="86"/>
+      <c r="D222" s="86"/>
+      <c r="E222" s="87"/>
       <c r="F222" s="18" t="s">
         <v>63</v>
       </c>
@@ -14130,12 +14180,12 @@
       <c r="A223" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B223" s="83" t="s">
+      <c r="B223" s="88" t="s">
         <v>241</v>
       </c>
-      <c r="C223" s="97"/>
-      <c r="D223" s="97"/>
-      <c r="E223" s="97"/>
+      <c r="C223" s="81"/>
+      <c r="D223" s="81"/>
+      <c r="E223" s="81"/>
       <c r="F223" s="21" t="s">
         <v>63</v>
       </c>
@@ -14180,11 +14230,11 @@
       <c r="C228" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D228" s="95" t="s">
+      <c r="D228" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="E228" s="95"/>
-      <c r="F228" s="95"/>
+      <c r="E228" s="76"/>
+      <c r="F228" s="76"/>
       <c r="G228" s="57"/>
     </row>
     <row r="229" spans="1:7">
@@ -14197,11 +14247,11 @@
       <c r="C229" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D229" s="107" t="s">
+      <c r="D229" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="E229" s="107"/>
-      <c r="F229" s="107"/>
+      <c r="E229" s="75"/>
+      <c r="F229" s="75"/>
       <c r="G229" s="41"/>
     </row>
     <row r="230" spans="1:7">
@@ -14214,11 +14264,11 @@
       <c r="C230" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D230" s="107" t="s">
+      <c r="D230" s="75" t="s">
         <v>245</v>
       </c>
-      <c r="E230" s="107"/>
-      <c r="F230" s="107"/>
+      <c r="E230" s="75"/>
+      <c r="F230" s="75"/>
       <c r="G230" s="41"/>
     </row>
     <row r="231" spans="1:7">
@@ -14231,11 +14281,11 @@
       <c r="C231" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D231" s="107" t="s">
+      <c r="D231" s="75" t="s">
         <v>246</v>
       </c>
-      <c r="E231" s="107"/>
-      <c r="F231" s="107"/>
+      <c r="E231" s="75"/>
+      <c r="F231" s="75"/>
       <c r="G231" s="41"/>
     </row>
     <row r="232" spans="1:7">
@@ -14248,11 +14298,11 @@
       <c r="C232" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D232" s="107" t="s">
+      <c r="D232" s="75" t="s">
         <v>247</v>
       </c>
-      <c r="E232" s="107"/>
-      <c r="F232" s="107"/>
+      <c r="E232" s="75"/>
+      <c r="F232" s="75"/>
       <c r="G232" s="41"/>
     </row>
     <row r="233" spans="1:7">
@@ -14265,11 +14315,11 @@
       <c r="C233" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D233" s="107" t="s">
+      <c r="D233" s="75" t="s">
         <v>248</v>
       </c>
-      <c r="E233" s="107"/>
-      <c r="F233" s="107"/>
+      <c r="E233" s="75"/>
+      <c r="F233" s="75"/>
       <c r="G233" s="41"/>
     </row>
     <row r="234" spans="1:7">
@@ -14282,11 +14332,11 @@
       <c r="C234" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D234" s="103" t="s">
+      <c r="D234" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="E234" s="104"/>
-      <c r="F234" s="105"/>
+      <c r="E234" s="72"/>
+      <c r="F234" s="73"/>
       <c r="G234" s="43"/>
     </row>
     <row r="235" spans="1:7">
@@ -14299,11 +14349,11 @@
       <c r="C235" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D235" s="103" t="s">
+      <c r="D235" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="E235" s="104"/>
-      <c r="F235" s="105"/>
+      <c r="E235" s="72"/>
+      <c r="F235" s="73"/>
       <c r="G235" s="43"/>
     </row>
     <row r="236" spans="1:7">
@@ -14316,11 +14366,11 @@
       <c r="C236" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D236" s="103" t="s">
+      <c r="D236" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="E236" s="104"/>
-      <c r="F236" s="105"/>
+      <c r="E236" s="72"/>
+      <c r="F236" s="73"/>
       <c r="G236" s="43"/>
     </row>
     <row r="237" spans="1:7">
@@ -14401,57 +14451,34 @@
       <c r="C241" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D241" s="106" t="s">
+      <c r="D241" s="74" t="s">
         <v>261</v>
       </c>
-      <c r="E241" s="106"/>
-      <c r="F241" s="106"/>
+      <c r="E241" s="74"/>
+      <c r="F241" s="74"/>
       <c r="G241" s="44"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ap+vydlQsTivses2kTOZJOfe+E+ofk18ovQVkbwX/cy/2QzQqNYlkd6ZRwhTqYv60tXLJj9O4rjHfeOPlaqbDA==" saltValue="NIz07f4XZ+x9XJy8gC1img==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="115" topLeftCell="A172">
       <selection activeCell="C180" sqref="C180"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="115" topLeftCell="A172">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <selection activeCell="C180" sqref="C180"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D241:F241"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D228:F228"/>
-    <mergeCell ref="A211:A214"/>
-    <mergeCell ref="B211:B212"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="B213:B214"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="B219:E219"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="A207:A210"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="C207:E207"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="B209:B210"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="B173:B175"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B147:B159"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="B162:B164"/>
+    <mergeCell ref="B165:B172"/>
     <mergeCell ref="B176:B177"/>
     <mergeCell ref="B178:B184"/>
     <mergeCell ref="C198:E198"/>
@@ -14468,12 +14495,35 @@
     <mergeCell ref="B205:B206"/>
     <mergeCell ref="C205:E205"/>
     <mergeCell ref="C206:E206"/>
-    <mergeCell ref="B173:B175"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B147:B159"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="B165:B172"/>
+    <mergeCell ref="A207:A210"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="B209:B210"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="D228:F228"/>
+    <mergeCell ref="A211:A214"/>
+    <mergeCell ref="B211:B212"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="B213:B214"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="B219:E219"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D241:F241"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -14496,18 +14546,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i450--dynamic update build data method update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/analysis_00_ta_engine.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/analysis_00_ta_engine.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{D896A32E-20EB-49EA-8A4D-C0B0B2E9CB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -27,16 +28,16 @@
   </definedNames>
   <calcPr calcId="122211" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
+    <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1" showComments="commIndAndComment"/>
-    <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="494">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1377,33 +1378,6 @@
     <t>SDC_cases/07_set_output_delay/wildcard_ports_01</t>
   </si>
   <si>
-    <t>84</t>
-  </si>
-  <si>
-    <t>IO_Timing</t>
-  </si>
-  <si>
-    <t>SDC_cases/14_new_feature/IO_timing/case3</t>
-  </si>
-  <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t>of_object</t>
-  </si>
-  <si>
-    <t>SDC_cases/14_new_feature/of_object</t>
-  </si>
-  <si>
-    <t>86</t>
-  </si>
-  <si>
-    <t>MPW</t>
-  </si>
-  <si>
-    <t>SDC_cases/14_new_feature/MPW/EBR</t>
-  </si>
-  <si>
     <t>87</t>
   </si>
   <si>
@@ -1570,12 +1544,18 @@
   </si>
   <si>
     <t>radiant=ng3_1</t>
+  </si>
+  <si>
+    <t>cmd = python DEV/bin/run_radiant.py --synthesis=lse --trace-report-format default;override=local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmd =python DEV/bin/run_radiant.py --synthesis=lse --trace-report-format default;override=local </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00_ "/>
     <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
@@ -2660,7 +2640,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2668,13 +2648,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47">
@@ -2734,7 +2714,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2770,22 +2750,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="41" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2815,22 +2786,16 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="49" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="15" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="16" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2845,13 +2810,13 @@
     <xf numFmtId="165" fontId="21" fillId="0" borderId="24" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="21" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2872,31 +2837,64 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2908,13 +2906,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2934,44 +2926,17 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -3008,19 +2973,19 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink 2" xfId="49"/>
+    <cellStyle name="Hyperlink 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="41"/>
-    <cellStyle name="Normal 2 2" xfId="47"/>
-    <cellStyle name="Normal 3" xfId="44"/>
-    <cellStyle name="Normal 4" xfId="45"/>
-    <cellStyle name="Normal 5" xfId="46"/>
-    <cellStyle name="Normal 6" xfId="43"/>
-    <cellStyle name="Normal 6 2" xfId="48"/>
-    <cellStyle name="Note 2" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 4" xfId="45" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 5" xfId="46" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 6" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 6 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Note 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
@@ -3056,7 +3021,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5172,7 +5143,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -5227,7 +5204,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5272,7 +5255,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5391,7 +5380,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5438,7 +5433,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5474,7 +5475,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4EC3B0E1-484D-4565-B55C-A338B512C93B}" diskRevisions="1" revisionId="770" version="14">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AD2EBB4C-439C-4785-BA96-D73E096C9B77}" diskRevisions="1" revisionId="775" version="17">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5587,6 +5588,30 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{80F0B67E-3D19-4A38-8678-A86ED15C185E}" dateTime="2023-03-06T15:02:38" maxSheetId="5" userName="Jason Wang" r:id="rId15" minRId="771">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{68A09A50-BADC-4DFB-B7E9-033CBE94DE9A}" dateTime="2023-03-06T15:03:23" maxSheetId="5" userName="Jason Wang" r:id="rId16" minRId="772">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AD2EBB4C-439C-4785-BA96-D73E096C9B77}" dateTime="2023-03-06T15:38:56" maxSheetId="5" userName="Jason Wang" r:id="rId17" minRId="773" maxRId="775">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -7236,6 +7261,163 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="771" sId="2">
+    <nc r="O98" t="inlineStr">
+      <is>
+        <t>cmd = python DEV/bin/run_radiant.py --synthesis=lse --trace-report-format default;override=local</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="772" sId="2">
+    <oc r="O48" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+      </is>
+    </oc>
+    <nc r="O48" t="inlineStr">
+      <is>
+        <t xml:space="preserve">cmd =python DEV/bin/run_radiant.py --synthesis=lse --trace-report-format default;override=local </t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="773" sId="2" ref="A86:XFD86" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A86:XFD86" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="30" formatCode="@"/>
+        <protection locked="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="A86" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="D86" t="inlineStr">
+        <is>
+          <t>IO_Timing</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="E86" t="inlineStr">
+        <is>
+          <t>SDC_cases/14_new_feature/IO_timing/case3</t>
+        </is>
+      </nc>
+    </rcc>
+    <rfmt sheetId="2" sqref="L86" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="0" formatCode="General"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="S86" t="inlineStr">
+        <is>
+          <t>Default</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rrc rId="774" sId="2" ref="A86:XFD86" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A86:XFD86" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="30" formatCode="@"/>
+        <protection locked="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="A86" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="D86" t="inlineStr">
+        <is>
+          <t>of_object</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="E86" t="inlineStr">
+        <is>
+          <t>SDC_cases/14_new_feature/of_object</t>
+        </is>
+      </nc>
+    </rcc>
+    <rfmt sheetId="2" sqref="L86" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="0" formatCode="General"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="S86" t="inlineStr">
+        <is>
+          <t>Default</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rrc rId="775" sId="2" ref="A86:XFD86" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A86:XFD86" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="30" formatCode="@"/>
+        <protection locked="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="A86" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="D86" t="inlineStr">
+        <is>
+          <t>MPW</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="E86" t="inlineStr">
+        <is>
+          <t>SDC_cases/14_new_feature/MPW/EBR</t>
+        </is>
+      </nc>
+    </rcc>
+    <rfmt sheetId="2" sqref="L86" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="0" formatCode="General"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="S86" t="inlineStr">
+        <is>
+          <t>Default</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="1" sId="1">
@@ -11322,7 +11504,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" name="Cherry (Ying) Xu" id="-707422276" dateTime="2020-11-23T15:52:35"/>
 </users>
@@ -11404,6 +11586,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -11439,6 +11638,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -11614,10 +11830,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -11647,7 +11865,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -11673,7 +11891,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -11681,7 +11899,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -11702,22 +11920,22 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
       <selection activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -11729,15 +11947,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD110"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AD107"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -11770,40 +11988,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="70" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
     </row>
     <row r="2" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -11908,10 +12126,10 @@
         <v>267</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -11925,10 +12143,10 @@
         <v>268</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -11942,10 +12160,10 @@
         <v>269</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -11959,10 +12177,10 @@
         <v>270</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -11976,10 +12194,10 @@
         <v>272</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -11993,10 +12211,10 @@
         <v>273</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -12010,10 +12228,10 @@
         <v>275</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -12027,10 +12245,10 @@
         <v>278</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -12044,10 +12262,10 @@
         <v>279</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -12061,10 +12279,10 @@
         <v>281</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -12078,10 +12296,10 @@
         <v>283</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="14" spans="1:30">
@@ -12095,10 +12313,10 @@
         <v>285</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -12112,10 +12330,10 @@
         <v>287</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -12129,10 +12347,10 @@
         <v>289</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -12146,10 +12364,10 @@
         <v>291</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -12163,10 +12381,10 @@
         <v>293</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -12180,10 +12398,10 @@
         <v>296</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -12197,10 +12415,10 @@
         <v>298</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="21" spans="1:19">
@@ -12214,10 +12432,10 @@
         <v>300</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -12231,10 +12449,10 @@
         <v>302</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -12248,10 +12466,10 @@
         <v>304</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -12265,10 +12483,10 @@
         <v>306</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -12282,10 +12500,10 @@
         <v>309</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -12299,10 +12517,10 @@
         <v>311</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="27" spans="1:19">
@@ -12316,10 +12534,10 @@
         <v>313</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="28" spans="1:19">
@@ -12333,10 +12551,10 @@
         <v>315</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="29" spans="1:19">
@@ -12350,10 +12568,10 @@
         <v>317</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -12367,10 +12585,10 @@
         <v>319</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="31" spans="1:19">
@@ -12384,10 +12602,10 @@
         <v>321</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="32" spans="1:19">
@@ -12401,10 +12619,10 @@
         <v>323</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="33" spans="1:19">
@@ -12418,10 +12636,10 @@
         <v>326</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="34" spans="1:19">
@@ -12435,10 +12653,10 @@
         <v>328</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="35" spans="1:19">
@@ -12452,10 +12670,10 @@
         <v>330</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="36" spans="1:19">
@@ -12469,10 +12687,10 @@
         <v>332</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="37" spans="1:19">
@@ -12486,10 +12704,10 @@
         <v>334</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="38" spans="1:19">
@@ -12503,10 +12721,10 @@
         <v>336</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="39" spans="1:19">
@@ -12520,10 +12738,10 @@
         <v>338</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="40" spans="1:19">
@@ -12537,10 +12755,10 @@
         <v>340</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="41" spans="1:19">
@@ -12554,10 +12772,10 @@
         <v>342</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="42" spans="1:19">
@@ -12571,10 +12789,10 @@
         <v>344</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="43" spans="1:19">
@@ -12588,10 +12806,10 @@
         <v>346</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="44" spans="1:19">
@@ -12605,10 +12823,10 @@
         <v>348</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="45" spans="1:19">
@@ -12622,10 +12840,10 @@
         <v>350</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="46" spans="1:19">
@@ -12639,10 +12857,10 @@
         <v>352</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="47" spans="1:19">
@@ -12656,10 +12874,10 @@
         <v>354</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="48" spans="1:19">
@@ -12673,10 +12891,10 @@
         <v>357</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="49" spans="1:19">
@@ -12690,10 +12908,10 @@
         <v>359</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="50" spans="1:19">
@@ -12707,10 +12925,10 @@
         <v>361</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="51" spans="1:19">
@@ -12724,10 +12942,10 @@
         <v>364</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="52" spans="1:19">
@@ -12741,10 +12959,10 @@
         <v>366</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S52" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="53" spans="1:19">
@@ -12758,10 +12976,10 @@
         <v>368</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S53" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="54" spans="1:19">
@@ -12775,10 +12993,10 @@
         <v>370</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S54" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="55" spans="1:19">
@@ -12792,10 +13010,10 @@
         <v>372</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S55" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="56" spans="1:19">
@@ -12809,10 +13027,10 @@
         <v>374</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S56" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="57" spans="1:19">
@@ -12826,10 +13044,10 @@
         <v>376</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S57" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="58" spans="1:19">
@@ -12843,10 +13061,10 @@
         <v>378</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S58" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="59" spans="1:19">
@@ -12860,10 +13078,10 @@
         <v>380</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S59" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="60" spans="1:19">
@@ -12877,10 +13095,10 @@
         <v>382</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S60" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="61" spans="1:19">
@@ -12894,10 +13112,10 @@
         <v>385</v>
       </c>
       <c r="O61" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S61" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="62" spans="1:19">
@@ -12911,10 +13129,10 @@
         <v>387</v>
       </c>
       <c r="O62" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S62" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="63" spans="1:19">
@@ -12928,10 +13146,10 @@
         <v>389</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S63" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="64" spans="1:19">
@@ -12945,10 +13163,10 @@
         <v>391</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S64" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="65" spans="1:19">
@@ -12962,10 +13180,10 @@
         <v>393</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S65" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="66" spans="1:19">
@@ -12979,10 +13197,10 @@
         <v>395</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S66" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="67" spans="1:19">
@@ -12996,10 +13214,10 @@
         <v>397</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S67" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="68" spans="1:19">
@@ -13013,10 +13231,10 @@
         <v>400</v>
       </c>
       <c r="O68" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S68" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="69" spans="1:19">
@@ -13030,10 +13248,10 @@
         <v>402</v>
       </c>
       <c r="O69" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S69" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="70" spans="1:19">
@@ -13047,10 +13265,10 @@
         <v>404</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S70" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="71" spans="1:19">
@@ -13064,10 +13282,10 @@
         <v>406</v>
       </c>
       <c r="O71" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S71" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="72" spans="1:19">
@@ -13081,10 +13299,10 @@
         <v>408</v>
       </c>
       <c r="O72" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S72" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="73" spans="1:19">
@@ -13098,10 +13316,10 @@
         <v>410</v>
       </c>
       <c r="O73" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S73" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="74" spans="1:19">
@@ -13115,10 +13333,10 @@
         <v>412</v>
       </c>
       <c r="O74" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S74" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="75" spans="1:19">
@@ -13132,10 +13350,10 @@
         <v>414</v>
       </c>
       <c r="O75" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S75" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="76" spans="1:19">
@@ -13149,10 +13367,10 @@
         <v>416</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S76" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="77" spans="1:19">
@@ -13166,10 +13384,10 @@
         <v>418</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S77" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="78" spans="1:19">
@@ -13183,10 +13401,10 @@
         <v>421</v>
       </c>
       <c r="O78" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S78" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="79" spans="1:19">
@@ -13200,10 +13418,10 @@
         <v>423</v>
       </c>
       <c r="O79" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S79" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="80" spans="1:19">
@@ -13217,10 +13435,10 @@
         <v>425</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S80" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="81" spans="1:19">
@@ -13234,10 +13452,10 @@
         <v>427</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S81" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="82" spans="1:19">
@@ -13251,10 +13469,10 @@
         <v>429</v>
       </c>
       <c r="O82" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S82" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="83" spans="1:19">
@@ -13268,10 +13486,10 @@
         <v>431</v>
       </c>
       <c r="O83" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S83" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="84" spans="1:19">
@@ -13285,10 +13503,10 @@
         <v>433</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S84" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="85" spans="1:19">
@@ -13302,10 +13520,10 @@
         <v>435</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="S85" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="86" spans="1:19">
@@ -13319,7 +13537,7 @@
         <v>438</v>
       </c>
       <c r="S86" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="87" spans="1:19">
@@ -13327,371 +13545,332 @@
         <v>439</v>
       </c>
       <c r="D87" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>441</v>
-      </c>
       <c r="S87" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="88" spans="1:19">
       <c r="A88" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>444</v>
-      </c>
       <c r="S88" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="89" spans="1:19">
       <c r="A89" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>447</v>
-      </c>
       <c r="S89" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="90" spans="1:19">
       <c r="A90" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S90" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="91" spans="1:19">
       <c r="A91" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="S91" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="92" spans="1:19">
       <c r="A92" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="S92" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="93" spans="1:19">
       <c r="A93" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>453</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="S93" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="94" spans="1:19">
       <c r="A94" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>453</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="S94" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="95" spans="1:19">
       <c r="A95" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>453</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
+      </c>
+      <c r="O95" s="2" t="s">
+        <v>492</v>
       </c>
       <c r="S95" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="96" spans="1:19">
       <c r="A96" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="S96" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="97" spans="1:19">
       <c r="A97" s="2" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D97" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="E97" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="E97" s="2" t="s">
-        <v>465</v>
-      </c>
       <c r="S97" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="98" spans="1:19">
       <c r="A98" s="2" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="S98" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="99" spans="1:19">
       <c r="A99" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="S99" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="100" spans="1:19">
       <c r="A100" s="2" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="S100" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="101" spans="1:19">
       <c r="A101" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="S101" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="102" spans="1:19">
       <c r="A102" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="S102" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="103" spans="1:19">
       <c r="A103" s="2" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="S103" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="104" spans="1:19">
       <c r="A104" s="2" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="S104" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="105" spans="1:19">
       <c r="A105" s="2" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="S105" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="106" spans="1:19">
       <c r="A106" s="2" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>462</v>
+        <v>480</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="S106" s="2" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="107" spans="1:19">
       <c r="A107" s="2" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>462</v>
+        <v>480</v>
       </c>
       <c r="E107" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="O107" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="S107" s="2" t="s">
         <v>485</v>
-      </c>
-      <c r="S107" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="108" spans="1:19">
-      <c r="A108" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="S108" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="109" spans="1:19">
-      <c r="A109" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="S109" s="2" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="110" spans="1:19">
-      <c r="A110" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="O110" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="S110" s="2" t="s">
-        <v>494</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="y+CBG6/YKaQ6HsaQYTqaGGAc9K7SdI4KYNN5n42I5k04yiTX0Fn8xQwrYnwNAtl9mwRmr3UcHPCrpySoPgBJNA==" saltValue="2QS/OSgjoJCpqDc5Ec8Idw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A2:AD2"/>
+  <autoFilter ref="A2:AD2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="70" showAutoFilter="1">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:AD2"/>
+      <autoFilter ref="A2:Y2" xr:uid="{BAC6815F-1A6E-4254-9FBF-BB2CC9945BCD}"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A2:Y2" xr:uid="{98BFEE33-43F6-4EB5-8DD3-7FF0F15C401A}"/>
     </customSheetView>
     <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="70" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="A109" sqref="A109:XFD109"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A2:AD2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <autoFilter ref="A2:AD2" xr:uid="{0C2116BD-4E09-4DF0-A947-8480F7773CF2}"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="70" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:Y2"/>
-    </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AD2" xr:uid="{B2B597B6-437A-4DCD-BB7F-5D35FCC4A807}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -13700,10 +13879,10 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1 W1:AA1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1 W1:AA1" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:V1 A1 C1:E1 G1:H1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:V1 A1 C1:E1 G1:H1" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$F$31:$J$31</formula1>
     </dataValidation>
   </dataValidations>
@@ -13712,49 +13891,49 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>description!$F$140:$H$140</xm:f>
           </x14:formula1>
           <xm:sqref>AB1:AB1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>description!$F$141:$H$141</xm:f>
           </x14:formula1>
           <xm:sqref>AC1:AC1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>description!$F$122:$H$122</xm:f>
           </x14:formula1>
           <xm:sqref>K1:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>description!$F$121:$K$121</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>description!$F$123:$H$123</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>description!$E$113:$F$113</xm:f>
           </x14:formula1>
           <xm:sqref>B1:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>description!$F$117:$H$117</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>description!$F$120:$K$120</xm:f>
           </x14:formula1>
@@ -13767,7 +13946,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N241"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -13832,17 +14011,17 @@
       <c r="E111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F111" s="73" t="s">
+      <c r="F111" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="G111" s="74"/>
-      <c r="H111" s="74"/>
-      <c r="I111" s="74"/>
-      <c r="J111" s="74"/>
-      <c r="K111" s="74"/>
-      <c r="L111" s="74"/>
-      <c r="M111" s="74"/>
-      <c r="N111" s="75"/>
+      <c r="G111" s="100"/>
+      <c r="H111" s="100"/>
+      <c r="I111" s="100"/>
+      <c r="J111" s="100"/>
+      <c r="K111" s="100"/>
+      <c r="L111" s="100"/>
+      <c r="M111" s="100"/>
+      <c r="N111" s="101"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -14706,7 +14885,7 @@
       <c r="A147" s="26">
         <v>1</v>
       </c>
-      <c r="B147" s="76" t="s">
+      <c r="B147" s="84" t="s">
         <v>3</v>
       </c>
       <c r="C147" s="27" t="s">
@@ -14732,7 +14911,7 @@
       <c r="A148" s="26">
         <v>2</v>
       </c>
-      <c r="B148" s="77"/>
+      <c r="B148" s="85"/>
       <c r="C148" s="28" t="s">
         <v>136</v>
       </c>
@@ -14754,7 +14933,7 @@
       <c r="A149" s="26">
         <v>3</v>
       </c>
-      <c r="B149" s="77"/>
+      <c r="B149" s="85"/>
       <c r="C149" s="28" t="s">
         <v>9</v>
       </c>
@@ -14774,7 +14953,7 @@
       <c r="A150" s="26">
         <v>4</v>
       </c>
-      <c r="B150" s="77"/>
+      <c r="B150" s="85"/>
       <c r="C150" s="28" t="s">
         <v>138</v>
       </c>
@@ -14798,7 +14977,7 @@
       <c r="A151" s="26">
         <v>5</v>
       </c>
-      <c r="B151" s="77"/>
+      <c r="B151" s="85"/>
       <c r="C151" s="27" t="s">
         <v>140</v>
       </c>
@@ -14822,7 +15001,7 @@
       <c r="A152" s="26">
         <v>6</v>
       </c>
-      <c r="B152" s="77"/>
+      <c r="B152" s="85"/>
       <c r="C152" s="27" t="s">
         <v>144</v>
       </c>
@@ -14846,7 +15025,7 @@
       <c r="A153" s="26">
         <v>7</v>
       </c>
-      <c r="B153" s="77"/>
+      <c r="B153" s="85"/>
       <c r="C153" s="28" t="s">
         <v>147</v>
       </c>
@@ -14868,7 +15047,7 @@
       <c r="A154" s="26">
         <v>8</v>
       </c>
-      <c r="B154" s="77"/>
+      <c r="B154" s="85"/>
       <c r="C154" s="27" t="s">
         <v>148</v>
       </c>
@@ -14892,7 +15071,7 @@
       <c r="A155" s="26">
         <v>9</v>
       </c>
-      <c r="B155" s="77"/>
+      <c r="B155" s="85"/>
       <c r="C155" s="27" t="s">
         <v>149</v>
       </c>
@@ -14916,7 +15095,7 @@
       <c r="A156" s="26">
         <v>10</v>
       </c>
-      <c r="B156" s="77"/>
+      <c r="B156" s="85"/>
       <c r="C156" s="28" t="s">
         <v>150</v>
       </c>
@@ -14940,7 +15119,7 @@
       <c r="A157" s="26">
         <v>11</v>
       </c>
-      <c r="B157" s="77"/>
+      <c r="B157" s="85"/>
       <c r="C157" s="28" t="s">
         <v>151</v>
       </c>
@@ -14964,7 +15143,7 @@
       <c r="A158" s="26">
         <v>12</v>
       </c>
-      <c r="B158" s="77"/>
+      <c r="B158" s="85"/>
       <c r="C158" s="28" t="s">
         <v>153</v>
       </c>
@@ -14986,7 +15165,7 @@
       <c r="A159" s="26">
         <v>13</v>
       </c>
-      <c r="B159" s="78"/>
+      <c r="B159" s="79"/>
       <c r="C159" s="28" t="s">
         <v>56</v>
       </c>
@@ -15010,7 +15189,7 @@
       <c r="A160" s="26">
         <v>14</v>
       </c>
-      <c r="B160" s="71" t="s">
+      <c r="B160" s="75" t="s">
         <v>4</v>
       </c>
       <c r="C160" s="28" t="s">
@@ -15036,7 +15215,7 @@
       <c r="A161" s="26">
         <v>15</v>
       </c>
-      <c r="B161" s="72"/>
+      <c r="B161" s="74"/>
       <c r="C161" s="28" t="s">
         <v>161</v>
       </c>
@@ -15060,7 +15239,7 @@
       <c r="A162" s="26">
         <v>16</v>
       </c>
-      <c r="B162" s="76" t="s">
+      <c r="B162" s="84" t="s">
         <v>5</v>
       </c>
       <c r="C162" s="28" t="s">
@@ -15084,7 +15263,7 @@
       <c r="A163" s="26">
         <v>17</v>
       </c>
-      <c r="B163" s="79"/>
+      <c r="B163" s="102"/>
       <c r="C163" s="27" t="s">
         <v>165</v>
       </c>
@@ -15106,7 +15285,7 @@
       <c r="A164" s="26">
         <v>18</v>
       </c>
-      <c r="B164" s="78"/>
+      <c r="B164" s="79"/>
       <c r="C164" s="27" t="s">
         <v>167</v>
       </c>
@@ -15126,7 +15305,7 @@
       <c r="A165" s="26">
         <v>19</v>
       </c>
-      <c r="B165" s="71" t="s">
+      <c r="B165" s="75" t="s">
         <v>6</v>
       </c>
       <c r="C165" s="28" t="s">
@@ -15150,7 +15329,7 @@
       <c r="A166" s="26">
         <v>20</v>
       </c>
-      <c r="B166" s="72"/>
+      <c r="B166" s="74"/>
       <c r="C166" s="28" t="s">
         <v>172</v>
       </c>
@@ -15170,7 +15349,7 @@
       <c r="A167" s="26">
         <v>21</v>
       </c>
-      <c r="B167" s="72"/>
+      <c r="B167" s="74"/>
       <c r="C167" s="28" t="s">
         <v>173</v>
       </c>
@@ -15190,7 +15369,7 @@
       <c r="A168" s="26">
         <v>22</v>
       </c>
-      <c r="B168" s="72"/>
+      <c r="B168" s="74"/>
       <c r="C168" s="28" t="s">
         <v>174</v>
       </c>
@@ -15210,7 +15389,7 @@
       <c r="A169" s="26">
         <v>23</v>
       </c>
-      <c r="B169" s="72"/>
+      <c r="B169" s="74"/>
       <c r="C169" s="28" t="s">
         <v>175</v>
       </c>
@@ -15230,7 +15409,7 @@
       <c r="A170" s="26">
         <v>24</v>
       </c>
-      <c r="B170" s="72"/>
+      <c r="B170" s="74"/>
       <c r="C170" s="28" t="s">
         <v>176</v>
       </c>
@@ -15250,7 +15429,7 @@
       <c r="A171" s="26">
         <v>25</v>
       </c>
-      <c r="B171" s="72"/>
+      <c r="B171" s="74"/>
       <c r="C171" s="28" t="s">
         <v>177</v>
       </c>
@@ -15270,7 +15449,7 @@
       <c r="A172" s="26">
         <v>26</v>
       </c>
-      <c r="B172" s="72"/>
+      <c r="B172" s="74"/>
       <c r="C172" s="28" t="s">
         <v>41</v>
       </c>
@@ -15290,7 +15469,7 @@
       <c r="A173" s="26">
         <v>27</v>
       </c>
-      <c r="B173" s="71" t="s">
+      <c r="B173" s="75" t="s">
         <v>7</v>
       </c>
       <c r="C173" s="28" t="s">
@@ -15314,7 +15493,7 @@
       <c r="A174" s="26">
         <v>28</v>
       </c>
-      <c r="B174" s="72"/>
+      <c r="B174" s="74"/>
       <c r="C174" s="27" t="s">
         <v>181</v>
       </c>
@@ -15336,7 +15515,7 @@
       <c r="A175" s="26">
         <v>29</v>
       </c>
-      <c r="B175" s="72"/>
+      <c r="B175" s="74"/>
       <c r="C175" s="28" t="s">
         <v>184</v>
       </c>
@@ -15358,7 +15537,7 @@
       <c r="A176" s="26">
         <v>30</v>
       </c>
-      <c r="B176" s="76" t="s">
+      <c r="B176" s="84" t="s">
         <v>8</v>
       </c>
       <c r="C176" s="28" t="s">
@@ -15384,7 +15563,7 @@
       <c r="A177" s="31">
         <v>31</v>
       </c>
-      <c r="B177" s="77"/>
+      <c r="B177" s="85"/>
       <c r="C177" s="32" t="s">
         <v>189</v>
       </c>
@@ -15408,7 +15587,7 @@
       <c r="A178" s="23">
         <v>32</v>
       </c>
-      <c r="B178" s="80" t="s">
+      <c r="B178" s="86" t="s">
         <v>191</v>
       </c>
       <c r="C178" s="33" t="s">
@@ -15432,7 +15611,7 @@
       <c r="A179" s="26">
         <v>33</v>
       </c>
-      <c r="B179" s="81"/>
+      <c r="B179" s="87"/>
       <c r="C179" s="27" t="s">
         <v>195</v>
       </c>
@@ -15454,7 +15633,7 @@
       <c r="A180" s="26">
         <v>34</v>
       </c>
-      <c r="B180" s="82"/>
+      <c r="B180" s="88"/>
       <c r="C180" s="34" t="s">
         <v>198</v>
       </c>
@@ -15476,7 +15655,7 @@
       <c r="A181" s="31">
         <v>35</v>
       </c>
-      <c r="B181" s="82"/>
+      <c r="B181" s="88"/>
       <c r="C181" s="34" t="s">
         <v>199</v>
       </c>
@@ -15498,17 +15677,17 @@
       <c r="A182" s="31">
         <v>36</v>
       </c>
-      <c r="B182" s="82"/>
+      <c r="B182" s="88"/>
       <c r="C182" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D182" s="42" t="s">
+      <c r="D182" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E182" s="42" t="s">
+      <c r="E182" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F182" s="42"/>
+      <c r="F182" s="32"/>
       <c r="G182" s="34" t="s">
         <v>260</v>
       </c>
@@ -15518,15 +15697,15 @@
       <c r="A183" s="31">
         <v>37</v>
       </c>
-      <c r="B183" s="82"/>
+      <c r="B183" s="88"/>
       <c r="C183" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="D183" s="42" t="s">
+      <c r="D183" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E183" s="42"/>
-      <c r="F183" s="42" t="s">
+      <c r="E183" s="32"/>
+      <c r="F183" s="32" t="s">
         <v>255</v>
       </c>
       <c r="G183" s="34" t="s">
@@ -15567,7 +15746,7 @@
       </c>
     </row>
     <row r="186" spans="1:8">
-      <c r="B186" s="37" t="s">
+      <c r="B186" s="6" t="s">
         <v>205</v>
       </c>
     </row>
@@ -15588,280 +15767,280 @@
       <c r="A198" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B198" s="38" t="s">
+      <c r="B198" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C198" s="84" t="s">
+      <c r="C198" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="D198" s="84"/>
-      <c r="E198" s="84"/>
-      <c r="F198" s="39" t="s">
+      <c r="D198" s="89"/>
+      <c r="E198" s="89"/>
+      <c r="F198" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="G198" s="40" t="s">
+      <c r="G198" s="38" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="199" spans="1:7">
-      <c r="A199" s="85" t="s">
+      <c r="A199" s="72" t="s">
         <v>212</v>
       </c>
-      <c r="B199" s="72" t="s">
+      <c r="B199" s="74" t="s">
         <v>213</v>
       </c>
-      <c r="C199" s="87" t="s">
+      <c r="C199" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="D199" s="88"/>
-      <c r="E199" s="88"/>
+      <c r="D199" s="92"/>
+      <c r="E199" s="92"/>
       <c r="F199" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G199" s="41" t="s">
+      <c r="G199" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="85"/>
-      <c r="B200" s="86"/>
-      <c r="C200" s="89" t="s">
+      <c r="A200" s="72"/>
+      <c r="B200" s="90"/>
+      <c r="C200" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="D200" s="90"/>
-      <c r="E200" s="90"/>
+      <c r="D200" s="94"/>
+      <c r="E200" s="94"/>
       <c r="F200" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="G200" s="43" t="s">
+      <c r="G200" s="40" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="85"/>
-      <c r="B201" s="72" t="s">
+      <c r="A201" s="72"/>
+      <c r="B201" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="C201" s="91" t="s">
+      <c r="C201" s="95" t="s">
         <v>217</v>
       </c>
-      <c r="D201" s="91"/>
-      <c r="E201" s="91"/>
+      <c r="D201" s="95"/>
+      <c r="E201" s="95"/>
       <c r="F201" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G201" s="41" t="s">
+      <c r="G201" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="85"/>
-      <c r="B202" s="72"/>
-      <c r="C202" s="89" t="s">
+      <c r="A202" s="72"/>
+      <c r="B202" s="74"/>
+      <c r="C202" s="93" t="s">
         <v>217</v>
       </c>
-      <c r="D202" s="89"/>
-      <c r="E202" s="89"/>
+      <c r="D202" s="93"/>
+      <c r="E202" s="93"/>
       <c r="F202" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G202" s="41" t="s">
+      <c r="G202" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="85"/>
-      <c r="B203" s="86" t="s">
+      <c r="A203" s="72"/>
+      <c r="B203" s="90" t="s">
         <v>218</v>
       </c>
-      <c r="C203" s="92" t="s">
+      <c r="C203" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="D203" s="93"/>
-      <c r="E203" s="94"/>
+      <c r="D203" s="97"/>
+      <c r="E203" s="98"/>
       <c r="F203" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G203" s="41" t="s">
+      <c r="G203" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="85"/>
-      <c r="B204" s="78"/>
-      <c r="C204" s="92" t="s">
+      <c r="A204" s="72"/>
+      <c r="B204" s="79"/>
+      <c r="C204" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="93"/>
-      <c r="E204" s="94"/>
+      <c r="D204" s="97"/>
+      <c r="E204" s="98"/>
       <c r="F204" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G204" s="41" t="s">
+      <c r="G204" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="85"/>
-      <c r="B205" s="72" t="s">
+      <c r="A205" s="72"/>
+      <c r="B205" s="74" t="s">
         <v>219</v>
       </c>
-      <c r="C205" s="91" t="s">
+      <c r="C205" s="95" t="s">
         <v>220</v>
       </c>
-      <c r="D205" s="91"/>
-      <c r="E205" s="91"/>
+      <c r="D205" s="95"/>
+      <c r="E205" s="95"/>
       <c r="F205" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G205" s="41" t="s">
+      <c r="G205" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="85"/>
-      <c r="B206" s="72"/>
-      <c r="C206" s="91" t="s">
+      <c r="A206" s="72"/>
+      <c r="B206" s="74"/>
+      <c r="C206" s="95" t="s">
         <v>220</v>
       </c>
-      <c r="D206" s="91"/>
-      <c r="E206" s="91"/>
+      <c r="D206" s="95"/>
+      <c r="E206" s="95"/>
       <c r="F206" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G206" s="41" t="s">
+      <c r="G206" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="85" t="s">
+      <c r="A207" s="72" t="s">
         <v>221</v>
       </c>
-      <c r="B207" s="72" t="s">
+      <c r="B207" s="74" t="s">
         <v>222</v>
       </c>
-      <c r="C207" s="71" t="s">
+      <c r="C207" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="D207" s="72"/>
-      <c r="E207" s="72"/>
+      <c r="D207" s="74"/>
+      <c r="E207" s="74"/>
       <c r="F207" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G207" s="41" t="s">
+      <c r="G207" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="85"/>
-      <c r="B208" s="72"/>
-      <c r="C208" s="72" t="s">
+      <c r="A208" s="72"/>
+      <c r="B208" s="74"/>
+      <c r="C208" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="D208" s="72"/>
-      <c r="E208" s="72"/>
+      <c r="D208" s="74"/>
+      <c r="E208" s="74"/>
       <c r="F208" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G208" s="41" t="s">
+      <c r="G208" s="39" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="85"/>
-      <c r="B209" s="72" t="s">
+      <c r="A209" s="72"/>
+      <c r="B209" s="74" t="s">
         <v>224</v>
       </c>
-      <c r="C209" s="72" t="s">
+      <c r="C209" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="D209" s="72"/>
-      <c r="E209" s="72"/>
+      <c r="D209" s="74"/>
+      <c r="E209" s="74"/>
       <c r="F209" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G209" s="41" t="s">
+      <c r="G209" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="85"/>
-      <c r="B210" s="72"/>
-      <c r="C210" s="72" t="s">
+      <c r="A210" s="72"/>
+      <c r="B210" s="74"/>
+      <c r="C210" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="D210" s="72"/>
-      <c r="E210" s="72"/>
+      <c r="D210" s="74"/>
+      <c r="E210" s="74"/>
       <c r="F210" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G210" s="41" t="s">
+      <c r="G210" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="85" t="s">
+      <c r="A211" s="72" t="s">
         <v>225</v>
       </c>
-      <c r="B211" s="72" t="s">
+      <c r="B211" s="74" t="s">
         <v>226</v>
       </c>
-      <c r="C211" s="71" t="s">
+      <c r="C211" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="D211" s="72"/>
-      <c r="E211" s="72"/>
+      <c r="D211" s="74"/>
+      <c r="E211" s="74"/>
       <c r="F211" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G211" s="41" t="s">
+      <c r="G211" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="85"/>
-      <c r="B212" s="72"/>
-      <c r="C212" s="72" t="s">
+      <c r="A212" s="72"/>
+      <c r="B212" s="74"/>
+      <c r="C212" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="D212" s="72"/>
-      <c r="E212" s="72"/>
+      <c r="D212" s="74"/>
+      <c r="E212" s="74"/>
       <c r="F212" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G212" s="41" t="s">
+      <c r="G212" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="85"/>
-      <c r="B213" s="72" t="s">
+      <c r="A213" s="72"/>
+      <c r="B213" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="C213" s="71" t="s">
+      <c r="C213" s="75" t="s">
         <v>228</v>
       </c>
-      <c r="D213" s="72"/>
-      <c r="E213" s="72"/>
+      <c r="D213" s="74"/>
+      <c r="E213" s="74"/>
       <c r="F213" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G213" s="41" t="s">
+      <c r="G213" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="214" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A214" s="96"/>
-      <c r="B214" s="97"/>
-      <c r="C214" s="97" t="s">
+      <c r="A214" s="73"/>
+      <c r="B214" s="76"/>
+      <c r="C214" s="76" t="s">
         <v>229</v>
       </c>
-      <c r="D214" s="97"/>
-      <c r="E214" s="97"/>
+      <c r="D214" s="76"/>
+      <c r="E214" s="76"/>
       <c r="F214" s="36" t="s">
         <v>215</v>
       </c>
-      <c r="G214" s="44" t="s">
+      <c r="G214" s="41" t="s">
         <v>63</v>
       </c>
     </row>
@@ -15869,60 +16048,43 @@
       <c r="A215" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C215" s="37"/>
-      <c r="D215" s="37"/>
-      <c r="E215" s="37"/>
-      <c r="F215" s="37"/>
-    </row>
-    <row r="216" spans="1:7">
-      <c r="C216" s="37"/>
-      <c r="D216" s="37"/>
-      <c r="E216" s="37"/>
-    </row>
-    <row r="217" spans="1:7">
-      <c r="C217" s="37"/>
-      <c r="D217" s="37"/>
-      <c r="E217" s="37"/>
     </row>
     <row r="218" spans="1:7" ht="15.75" thickBot="1">
       <c r="A218" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C218" s="37"/>
-      <c r="D218" s="37"/>
-      <c r="E218" s="37"/>
     </row>
     <row r="219" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A219" s="45" t="s">
+      <c r="A219" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="B219" s="98" t="s">
+      <c r="B219" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="C219" s="98"/>
-      <c r="D219" s="98"/>
-      <c r="E219" s="98"/>
-      <c r="F219" s="46" t="s">
+      <c r="C219" s="77"/>
+      <c r="D219" s="77"/>
+      <c r="E219" s="77"/>
+      <c r="F219" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="G219" s="47" t="s">
+      <c r="G219" s="44" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="93" customHeight="1">
-      <c r="A220" s="48" t="s">
+      <c r="A220" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="B220" s="99" t="s">
+      <c r="B220" s="78" t="s">
         <v>236</v>
       </c>
-      <c r="C220" s="78"/>
-      <c r="D220" s="78"/>
-      <c r="E220" s="78"/>
-      <c r="F220" s="49" t="s">
+      <c r="C220" s="79"/>
+      <c r="D220" s="79"/>
+      <c r="E220" s="79"/>
+      <c r="F220" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="G220" s="50" t="s">
+      <c r="G220" s="47" t="s">
         <v>63</v>
       </c>
     </row>
@@ -15930,12 +16092,12 @@
       <c r="A221" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B221" s="100" t="s">
+      <c r="B221" s="80" t="s">
         <v>238</v>
       </c>
-      <c r="C221" s="101"/>
-      <c r="D221" s="101"/>
-      <c r="E221" s="102"/>
+      <c r="C221" s="81"/>
+      <c r="D221" s="81"/>
+      <c r="E221" s="82"/>
       <c r="F221" s="15" t="s">
         <v>63</v>
       </c>
@@ -15947,12 +16109,12 @@
       <c r="A222" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B222" s="100" t="s">
+      <c r="B222" s="80" t="s">
         <v>239</v>
       </c>
-      <c r="C222" s="101"/>
-      <c r="D222" s="101"/>
-      <c r="E222" s="102"/>
+      <c r="C222" s="81"/>
+      <c r="D222" s="81"/>
+      <c r="E222" s="82"/>
       <c r="F222" s="18" t="s">
         <v>63</v>
       </c>
@@ -15967,9 +16129,9 @@
       <c r="B223" s="83" t="s">
         <v>241</v>
       </c>
-      <c r="C223" s="97"/>
-      <c r="D223" s="97"/>
-      <c r="E223" s="97"/>
+      <c r="C223" s="76"/>
+      <c r="D223" s="76"/>
+      <c r="E223" s="76"/>
       <c r="F223" s="21" t="s">
         <v>63</v>
       </c>
@@ -15978,7 +16140,7 @@
       </c>
     </row>
     <row r="224" spans="1:7">
-      <c r="C224" s="51"/>
+      <c r="C224" s="48"/>
     </row>
     <row r="226" spans="1:7" ht="15.75" thickBot="1">
       <c r="A226" s="6" t="s">
@@ -15989,303 +16151,280 @@
       <c r="A227" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="B227" s="38" t="s">
+      <c r="B227" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C227" s="52" t="s">
+      <c r="C227" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D227" s="53" t="s">
+      <c r="D227" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E227" s="53"/>
-      <c r="F227" s="54"/>
-      <c r="G227" s="40" t="s">
+      <c r="E227" s="50"/>
+      <c r="F227" s="10"/>
+      <c r="G227" s="38" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="228" spans="1:7">
-      <c r="A228" s="55">
+      <c r="A228" s="51">
         <v>42682</v>
       </c>
-      <c r="B228" s="56">
+      <c r="B228" s="52">
         <v>1.04</v>
       </c>
       <c r="C228" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D228" s="95" t="s">
+      <c r="D228" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="E228" s="95"/>
-      <c r="F228" s="95"/>
-      <c r="G228" s="57"/>
+      <c r="E228" s="71"/>
+      <c r="F228" s="71"/>
+      <c r="G228" s="25"/>
     </row>
     <row r="229" spans="1:7">
-      <c r="A229" s="58">
+      <c r="A229" s="53">
         <v>42692</v>
       </c>
-      <c r="B229" s="59">
+      <c r="B229" s="54">
         <v>1.05</v>
       </c>
       <c r="C229" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D229" s="107" t="s">
+      <c r="D229" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="E229" s="107"/>
-      <c r="F229" s="107"/>
-      <c r="G229" s="41"/>
+      <c r="E229" s="70"/>
+      <c r="F229" s="70"/>
+      <c r="G229" s="39"/>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="58">
+      <c r="A230" s="53">
         <v>42955</v>
       </c>
-      <c r="B230" s="59">
+      <c r="B230" s="54">
         <v>1.06</v>
       </c>
       <c r="C230" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D230" s="107" t="s">
+      <c r="D230" s="70" t="s">
         <v>245</v>
       </c>
-      <c r="E230" s="107"/>
-      <c r="F230" s="107"/>
-      <c r="G230" s="41"/>
+      <c r="E230" s="70"/>
+      <c r="F230" s="70"/>
+      <c r="G230" s="39"/>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="58">
+      <c r="A231" s="53">
         <v>42991</v>
       </c>
-      <c r="B231" s="59">
+      <c r="B231" s="54">
         <v>1.07</v>
       </c>
       <c r="C231" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D231" s="107" t="s">
+      <c r="D231" s="70" t="s">
         <v>246</v>
       </c>
-      <c r="E231" s="107"/>
-      <c r="F231" s="107"/>
-      <c r="G231" s="41"/>
+      <c r="E231" s="70"/>
+      <c r="F231" s="70"/>
+      <c r="G231" s="39"/>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="58">
+      <c r="A232" s="53">
         <v>43026</v>
       </c>
-      <c r="B232" s="59">
+      <c r="B232" s="54">
         <v>1.08</v>
       </c>
       <c r="C232" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D232" s="107" t="s">
+      <c r="D232" s="70" t="s">
         <v>247</v>
       </c>
-      <c r="E232" s="107"/>
-      <c r="F232" s="107"/>
-      <c r="G232" s="41"/>
+      <c r="E232" s="70"/>
+      <c r="F232" s="70"/>
+      <c r="G232" s="39"/>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="58">
+      <c r="A233" s="53">
         <v>43069</v>
       </c>
-      <c r="B233" s="59">
+      <c r="B233" s="54">
         <v>1.0900000000000001</v>
       </c>
       <c r="C233" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D233" s="107" t="s">
+      <c r="D233" s="70" t="s">
         <v>248</v>
       </c>
-      <c r="E233" s="107"/>
-      <c r="F233" s="107"/>
-      <c r="G233" s="41"/>
+      <c r="E233" s="70"/>
+      <c r="F233" s="70"/>
+      <c r="G233" s="39"/>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="60">
+      <c r="A234" s="55">
         <v>43248</v>
       </c>
-      <c r="B234" s="61">
+      <c r="B234" s="56">
         <v>1.1000000000000001</v>
       </c>
       <c r="C234" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D234" s="103" t="s">
+      <c r="D234" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="E234" s="104"/>
-      <c r="F234" s="105"/>
-      <c r="G234" s="43"/>
+      <c r="E234" s="67"/>
+      <c r="F234" s="68"/>
+      <c r="G234" s="40"/>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="60">
+      <c r="A235" s="55">
         <v>43339</v>
       </c>
-      <c r="B235" s="61">
+      <c r="B235" s="56">
         <v>1.1100000000000001</v>
       </c>
       <c r="C235" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D235" s="103" t="s">
+      <c r="D235" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="E235" s="104"/>
-      <c r="F235" s="105"/>
-      <c r="G235" s="43"/>
+      <c r="E235" s="67"/>
+      <c r="F235" s="68"/>
+      <c r="G235" s="40"/>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="60">
+      <c r="A236" s="55">
         <v>43542</v>
       </c>
-      <c r="B236" s="61">
+      <c r="B236" s="56">
         <v>1.1200000000000001</v>
       </c>
       <c r="C236" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D236" s="103" t="s">
+      <c r="D236" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="E236" s="104"/>
-      <c r="F236" s="105"/>
-      <c r="G236" s="43"/>
+      <c r="E236" s="67"/>
+      <c r="F236" s="68"/>
+      <c r="G236" s="40"/>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="60">
+      <c r="A237" s="55">
         <v>43599</v>
       </c>
-      <c r="B237" s="61">
+      <c r="B237" s="56">
         <v>1.1299999999999999</v>
       </c>
       <c r="C237" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D237" s="62" t="s">
+      <c r="D237" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="E237" s="63"/>
-      <c r="F237" s="64"/>
-      <c r="G237" s="43"/>
+      <c r="E237" s="58"/>
+      <c r="F237" s="59"/>
+      <c r="G237" s="40"/>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="60">
+      <c r="A238" s="55">
         <v>43643</v>
       </c>
-      <c r="B238" s="61">
+      <c r="B238" s="56">
         <v>1.1399999999999999</v>
       </c>
       <c r="C238" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D238" s="62" t="s">
+      <c r="D238" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="E238" s="63"/>
-      <c r="F238" s="64"/>
-      <c r="G238" s="43"/>
+      <c r="E238" s="58"/>
+      <c r="F238" s="59"/>
+      <c r="G238" s="40"/>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="60">
+      <c r="A239" s="55">
         <v>43894</v>
       </c>
-      <c r="B239" s="61">
+      <c r="B239" s="56">
         <v>1.1499999999999999</v>
       </c>
       <c r="C239" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D239" s="62" t="s">
+      <c r="D239" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="E239" s="63"/>
-      <c r="F239" s="64"/>
-      <c r="G239" s="43"/>
+      <c r="E239" s="58"/>
+      <c r="F239" s="59"/>
+      <c r="G239" s="40"/>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="60">
+      <c r="A240" s="55">
         <v>44017</v>
       </c>
-      <c r="B240" s="61">
+      <c r="B240" s="56">
         <v>1.1599999999999999</v>
       </c>
-      <c r="C240" s="42" t="s">
+      <c r="C240" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D240" s="62" t="s">
+      <c r="D240" s="57" t="s">
         <v>249</v>
       </c>
-      <c r="E240" s="63"/>
-      <c r="F240" s="64"/>
-      <c r="G240" s="43"/>
+      <c r="E240" s="58"/>
+      <c r="F240" s="59"/>
+      <c r="G240" s="40"/>
     </row>
     <row r="241" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A241" s="65">
+      <c r="A241" s="60">
         <v>44118</v>
       </c>
-      <c r="B241" s="66">
+      <c r="B241" s="61">
         <v>1.17</v>
       </c>
       <c r="C241" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D241" s="106" t="s">
+      <c r="D241" s="69" t="s">
         <v>261</v>
       </c>
-      <c r="E241" s="106"/>
-      <c r="F241" s="106"/>
-      <c r="G241" s="44"/>
+      <c r="E241" s="69"/>
+      <c r="F241" s="69"/>
+      <c r="G241" s="41"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ap+vydlQsTivses2kTOZJOfe+E+ofk18ovQVkbwX/cy/2QzQqNYlkd6ZRwhTqYv60tXLJj9O4rjHfeOPlaqbDA==" saltValue="NIz07f4XZ+x9XJy8gC1img==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="115" topLeftCell="A172">
       <selection activeCell="C180" sqref="C180"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="115" topLeftCell="A172">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <selection activeCell="C180" sqref="C180"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D241:F241"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D228:F228"/>
-    <mergeCell ref="A211:A214"/>
-    <mergeCell ref="B211:B212"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="B213:B214"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="B219:E219"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="A207:A210"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="C207:E207"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="B209:B210"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="B173:B175"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B147:B159"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="B162:B164"/>
+    <mergeCell ref="B165:B172"/>
     <mergeCell ref="B176:B177"/>
     <mergeCell ref="B178:B184"/>
     <mergeCell ref="C198:E198"/>
@@ -16302,12 +16441,35 @@
     <mergeCell ref="B205:B206"/>
     <mergeCell ref="C205:E205"/>
     <mergeCell ref="C206:E206"/>
-    <mergeCell ref="B173:B175"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B147:B159"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="B165:B172"/>
+    <mergeCell ref="A207:A210"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="B209:B210"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="D228:F228"/>
+    <mergeCell ref="A211:A214"/>
+    <mergeCell ref="B211:B212"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="B213:B214"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="B219:E219"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D241:F241"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -16316,7 +16478,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16330,18 +16492,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>